<commit_message>
Automatically handle population types for framework plots
</commit_message>
<xml_diff>
--- a/atomica/library/combined_framework.xlsx
+++ b/atomica/library/combined_framework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F72EB13-1A6D-436B-96CC-C5586986239D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47AAA4B-3D23-4CAE-ADD2-2D283BC3B9A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="2400" windowWidth="28065" windowHeight="17190" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7740" yWindow="2400" windowWidth="28065" windowHeight="17190" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Characteristics" sheetId="5" r:id="rId7"/>
     <sheet name="Parameters" sheetId="6" r:id="rId8"/>
     <sheet name="Cascades" sheetId="7" r:id="rId9"/>
+    <sheet name="Plots" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -754,8 +755,45 @@
 </comments>
 </file>
 
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>None</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{4E0A6107-2F83-4B61-AE65-8487AD3B3661}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>This column is for the 'display name' of a compartment within a
+population cascade, a state that an entity can exist in that is
+distinct from all other states.
+Examples may include 'Susceptible', 'Infected Stage 1', 'Recovered',
+etc.
+If entities in the network involve two 'orthogonal' descriptors,
+compartments should combine the status of each state in the title,
+e.g. 'High Income Earner + Year 12 Education', to make sure that each
+entity in a cascade is only ever in one state at a time.
+It is possible to bundle independent states as analytical features of
+interest elsewhere in the framework file.
+Note: A display name is a representative label that users interface
+with (e.g. in databooks and plots).
+It should be in title or sentence case.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="138">
   <si>
     <t>Name</t>
   </si>
@@ -1148,6 +1186,27 @@
   </si>
   <si>
     <t>udt_cascade</t>
+  </si>
+  <si>
+    <t>Quantities</t>
+  </si>
+  <si>
+    <t>SIR total</t>
+  </si>
+  <si>
+    <t>UDT total</t>
+  </si>
+  <si>
+    <t>SIR dict</t>
+  </si>
+  <si>
+    <t>SIR function</t>
+  </si>
+  <si>
+    <t>{'alive':['sus','inf','rec']}</t>
+  </si>
+  <si>
+    <t>{'alive':'sus+inf+rec'}</t>
   </si>
 </sst>
 </file>
@@ -1262,14 +1321,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -1682,6 +1734,66 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ACC3CA1-B25B-46ED-AC21-946C8547442C}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B11"/>
@@ -1761,7 +1873,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:B5">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>AND(A4&lt;&gt;"",NOT(B4&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1775,7 +1887,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:I7"/>
+      <selection activeCell="A4" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2089,7 +2201,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B7:B9">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>AND(A7&lt;&gt;"",NOT(B7&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2108,7 +2220,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2539,7 +2651,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3026,12 +3138,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>AND(A11&lt;&gt;"",NOT(B11&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C13">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND(#REF!&lt;&gt;"",NOT(C11&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3453,12 +3565,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10:B15">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND(A10&lt;&gt;"",NOT(B10&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D14">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND(#REF!&lt;&gt;"",NOT(D10&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3479,7 +3591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>

</xml_diff>